<commit_message>
Meziportletová komunikace, alloy UI
</commit_message>
<xml_diff>
--- a/rozvržení osnova strany.xlsx
+++ b/rozvržení osnova strany.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="27795" windowHeight="12075"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="23520" windowHeight="9450"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -129,12 +129,18 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,12 +155,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
@@ -461,7 +474,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,34 +492,34 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>4</v>
       </c>
     </row>
@@ -612,50 +625,50 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="4">
         <v>2</v>
       </c>
     </row>

</xml_diff>